<commit_message>
Alarm library doc updated
</commit_message>
<xml_diff>
--- a/PLC/90_Library/Alarm/__doc__.xlsx
+++ b/PLC/90_Library/Alarm/__doc__.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.0.2\work\PlcFramework\PLC\90_Library\Alarm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCFBB9B-A322-4B9B-B3E2-53D86750C241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B94831-4B45-42F1-B49F-372ED3E9CE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{68167A51-26E3-4450-BADD-375455D19BCB}"/>
   </bookViews>
   <sheets>
     <sheet name="CallHierarchy" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CallHierarchy!$A$2:$AJ$24</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="35">
   <si>
     <t>Object</t>
   </si>
@@ -136,9 +139,6 @@
     </r>
   </si>
   <si>
-    <t>_alarmTraceSuperUpdater</t>
-  </si>
-  <si>
     <t>alarmTraceSuperData[]</t>
   </si>
   <si>
@@ -163,9 +163,6 @@
   </si>
   <si>
     <t>_alarmTraceGlobalUpdater</t>
-  </si>
-  <si>
-    <t>_alarmTraceGlobalCollector(superId)</t>
   </si>
   <si>
     <r>
@@ -705,13 +702,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD51FD1-3261-4688-8B6C-01E560767421}">
-  <dimension ref="A1:AJ31"/>
+  <dimension ref="A1:AJ26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Z4" sqref="Z4"/>
+      <selection pane="bottomRight" activeCell="AK6" sqref="AK6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,7 +752,7 @@
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
       <c r="Z1" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA1" s="13"/>
       <c r="AB1" s="13"/>
@@ -848,7 +845,7 @@
         <v>2</v>
       </c>
       <c r="AA2" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB2" s="14" t="s">
         <v>17</v>
@@ -860,7 +857,7 @@
         <v>4</v>
       </c>
       <c r="AE2" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AF2" s="14" t="s">
         <v>20</v>
@@ -892,10 +889,10 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -954,7 +951,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>13</v>
@@ -963,10 +960,10 @@
         <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -1050,7 +1047,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>13</v>
@@ -1240,7 +1237,7 @@
         <v>24</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="11" t="s">
@@ -1380,7 +1377,7 @@
         <v>24</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="11"/>
@@ -1429,10 +1426,10 @@
         <v>13</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="11"/>
@@ -1521,7 +1518,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>13</v>
@@ -1668,7 +1665,7 @@
         <v>24</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="11"/>
@@ -1806,7 +1803,7 @@
         <v>24</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="11"/>
@@ -1855,10 +1852,10 @@
         <v>13</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="11"/>
@@ -1966,36 +1963,10 @@
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="E27" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="E28" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="E29" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="E30" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="E31" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="E26" s="15"/>
     </row>
   </sheetData>
+  <autoFilter ref="A2:AJ24" xr:uid="{2AD51FD1-3261-4688-8B6C-01E560767421}"/>
   <mergeCells count="3">
     <mergeCell ref="H1:N1"/>
     <mergeCell ref="P1:X1"/>

</xml_diff>